<commit_message>
Continued progress on blog includes integration of data from previous
</commit_message>
<xml_diff>
--- a/blog/flight data.xlsx
+++ b/blog/flight data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seths\Google Drive\Flatiron School\Blog posts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seths\Development\module1_project\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -299,25 +299,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.14746770771095388</c:v>
+                  <c:v>0.14282964644538773</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1441167663683954</c:v>
+                  <c:v>0.13958409679491798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15492911436865278</c:v>
+                  <c:v>0.1500563816503131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12552903981973695</c:v>
+                  <c:v>0.15303234851850808</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14687524674139998</c:v>
+                  <c:v>0.14225581918430399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15004315705449064</c:v>
+                  <c:v>0.14532409438172084</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13103896793637035</c:v>
+                  <c:v>0.12691761302484827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,25 +388,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.16635563200492673</c:v>
+                  <c:v>0.15876913437632789</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14464066452754973</c:v>
+                  <c:v>0.13804445828426054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15789550836767349</c:v>
+                  <c:v>0.15069482699992581</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12440908786493432</c:v>
+                  <c:v>0.16433961680752307</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13081444873405695</c:v>
+                  <c:v>0.12484877451463532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13240948599806115</c:v>
+                  <c:v>0.12637107155172289</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14347517250279762</c:v>
+                  <c:v>0.13693211746560449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1457,9 +1457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,11 +1519,11 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D4" si="0">IF(WEEKDAY(A2)=1, "Sun", IF(WEEKDAY(A2)=2, "Mon", IF(WEEKDAY(A2)=3, "Tue", IF(WEEKDAY(A2)=4, "Wed", IF(WEEKDAY(A2)=5,"Thu", IF(WEEKDAY(A2)=6, "Fri", IF(WEEKDAY(A2)=7, "Sat")))))))</f>
+        <f t="shared" ref="D2:D3" si="0">IF(WEEKDAY(A2)=1, "Sun", IF(WEEKDAY(A2)=2, "Mon", IF(WEEKDAY(A2)=3, "Tue", IF(WEEKDAY(A2)=4, "Wed", IF(WEEKDAY(A2)=5,"Thu", IF(WEEKDAY(A2)=6, "Fri", IF(WEEKDAY(A2)=7, "Sat")))))))</f>
         <v>Thu</v>
       </c>
       <c r="E2" s="5">
-        <f t="shared" ref="E2:E4" si="1">DATE(2020,12,30)-A2</f>
+        <f t="shared" ref="E2:E3" si="1">DATE(2020,12,30)-A2</f>
         <v>-1</v>
       </c>
       <c r="F2" s="5"/>
@@ -1533,27 +1533,31 @@
       </c>
       <c r="L2" s="6">
         <f>SUMIFS(B:B, $D:$D, $K2, $E:$E, "&lt;"&amp;$J$12)/SUMIFS(B:B, $E:$E, "&lt;"&amp;$J$12)</f>
-        <v>0.16635563200492673</v>
+        <v>0.15876913437632789</v>
       </c>
       <c r="M2" s="6">
         <f t="shared" ref="M2:M8" si="2">SUMIFS(C:C, $D:$D, $K2, $E:$E, "&lt;"&amp;$J$12)/SUMIFS(C:C, $E:$E, "&lt;"&amp;$J$12)</f>
-        <v>0.14746770771095388</v>
+        <v>0.14282964644538773</v>
       </c>
       <c r="N2" s="7">
         <f>L2/MAX(L$2:L$8)</f>
-        <v>1</v>
+        <v>0.96610383704545566</v>
       </c>
       <c r="O2" s="7">
         <f t="shared" ref="O2:O8" si="3">M2/MAX(M$2:M$8)</f>
-        <v>0.95183986761878381</v>
+        <v>0.93332976869340534</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44195</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3">
+        <v>1163696</v>
+      </c>
+      <c r="C3">
+        <v>2133253</v>
+      </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
@@ -1567,19 +1571,19 @@
       </c>
       <c r="L3" s="6">
         <f t="shared" ref="L3:L8" si="4">SUMIFS(B:B, $D:$D, $K3, $E:$E, "&lt;"&amp;$J$12)/SUMIFS(B:B, $E:$E, "&lt;"&amp;$J$12)</f>
-        <v>0.14464066452754973</v>
+        <v>0.13804445828426054</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="2"/>
-        <v>0.1441167663683954</v>
+        <v>0.13958409679491798</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" ref="N3:N8" si="5">L3/MAX(L$2:L$8)</f>
-        <v>0.86946659265053383</v>
+        <v>0.83999501134251886</v>
       </c>
       <c r="O3" s="7">
         <f t="shared" si="3"/>
-        <v>0.93021099975741506</v>
+        <v>0.91212150990440011</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1605,19 +1609,19 @@
       </c>
       <c r="L4" s="6">
         <f t="shared" si="4"/>
-        <v>0.15789550836767349</v>
+        <v>0.15069482699992581</v>
       </c>
       <c r="M4" s="6">
         <f t="shared" si="2"/>
-        <v>0.15492911436865278</v>
+        <v>0.1500563816503131</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="5"/>
-        <v>0.94914435095889815</v>
+        <v>0.91697199937141005</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.98055334772677116</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1643,19 +1647,19 @@
       </c>
       <c r="L5" s="6">
         <f t="shared" si="4"/>
-        <v>0.12440908786493432</v>
+        <v>0.16433961680752307</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="2"/>
-        <v>0.12552903981973695</v>
+        <v>0.15303234851850808</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="5"/>
-        <v>0.74785017113968144</v>
+        <v>1</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="3"/>
-        <v>0.81023531523611148</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1681,19 +1685,19 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" si="4"/>
-        <v>0.13081444873405695</v>
+        <v>0.12484877451463532</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>0.14687524674139998</v>
+        <v>0.14225581918430399</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="5"/>
-        <v>0.78635419286665809</v>
+        <v>0.75969980300526074</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" si="3"/>
-        <v>0.94801578993029889</v>
+        <v>0.92958005651399411</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1719,19 +1723,19 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="4"/>
-        <v>0.13240948599806115</v>
+        <v>0.12637107155172289</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>0.15004315705449064</v>
+        <v>0.14532409438172084</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="5"/>
-        <v>0.79594230987105841</v>
+        <v>0.76896291963325258</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="3"/>
-        <v>0.96846327216112504</v>
+        <v>0.94962990366801436</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1757,19 +1761,19 @@
       </c>
       <c r="L8" s="6">
         <f t="shared" si="4"/>
-        <v>0.14347517250279762</v>
+        <v>0.13693211746560449</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="2"/>
-        <v>0.13103896793637035</v>
+        <v>0.12691761302484827</v>
       </c>
       <c r="N8" s="7">
         <f t="shared" si="5"/>
-        <v>0.86246056579886943</v>
+        <v>0.83322646191868244</v>
       </c>
       <c r="O8" s="7">
         <f t="shared" si="3"/>
-        <v>0.84579950302022644</v>
+        <v>0.8293515341921226</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>